<commit_message>
Creating special classes to handle the different types of cards
</commit_message>
<xml_diff>
--- a/Monopoly_data.xlsx
+++ b/Monopoly_data.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Desktop\CS projects\Projects Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Desktop\CS projects\Python_Programs\github_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C03AEC-F69E-4AA7-A893-C76DD266137D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F642531-A545-4A80-BFE2-86C0E67BAF2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D6DA0972-7B55-441C-8D73-5E4A5A098029}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D6DA0972-7B55-441C-8D73-5E4A5A098029}"/>
   </bookViews>
   <sheets>
     <sheet name="European Cities" sheetId="1" r:id="rId1"/>
+    <sheet name="Special Cards" sheetId="2" r:id="rId2"/>
+    <sheet name="Transportation" sheetId="3" r:id="rId3"/>
+    <sheet name="Energy" sheetId="4" r:id="rId4"/>
+    <sheet name="Community Cards" sheetId="5" r:id="rId5"/>
+    <sheet name="Chance Cards" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>City</t>
   </si>
@@ -118,6 +123,129 @@
   </si>
   <si>
     <t>Nicosia</t>
+  </si>
+  <si>
+    <t>Starting Point</t>
+  </si>
+  <si>
+    <t>Visit Prison</t>
+  </si>
+  <si>
+    <t>Free Holidays</t>
+  </si>
+  <si>
+    <t>Go to Jail</t>
+  </si>
+  <si>
+    <t>Hydro Electric</t>
+  </si>
+  <si>
+    <t>Wind Electricity</t>
+  </si>
+  <si>
+    <t>Paris to Bourdeux</t>
+  </si>
+  <si>
+    <t>Coppenhagen to Malmo</t>
+  </si>
+  <si>
+    <t>London to Garforth</t>
+  </si>
+  <si>
+    <t>Vienna to Walserberg</t>
+  </si>
+  <si>
+    <t>Money Get</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Money Lost</t>
+  </si>
+  <si>
+    <t>Income Tax</t>
+  </si>
+  <si>
+    <t>Super Tax</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Advance to the starting point</t>
+  </si>
+  <si>
+    <t>Bank Error: You get 200,000 from the Bank</t>
+  </si>
+  <si>
+    <t>Get out of jail free card</t>
+  </si>
+  <si>
+    <t>Go to prison without passig through the starting point</t>
+  </si>
+  <si>
+    <t>School fees: Pay 50,000 for school tuition</t>
+  </si>
+  <si>
+    <t>You have won the 2nd place in an ugliness competition. Get 10,000</t>
+  </si>
+  <si>
+    <t>You inherit 100,000 from your aunt</t>
+  </si>
+  <si>
+    <t>Grand Opera! You need a new tux. Pay 20,000</t>
+  </si>
+  <si>
+    <t>Happy birthday, get 20,000 from each player</t>
+  </si>
+  <si>
+    <t>Life Insurance: Collect 50,000 from the bank</t>
+  </si>
+  <si>
+    <t>Take a walk. Advance 5 blocks</t>
+  </si>
+  <si>
+    <t>Bank offers you dividends. Collect 20,000</t>
+  </si>
+  <si>
+    <t>Pay poor taxes of 25,000</t>
+  </si>
+  <si>
+    <t>Go to jail without passing from the starting point</t>
+  </si>
+  <si>
+    <t>Go back 3 boxes</t>
+  </si>
+  <si>
+    <t>Your houses collapsed. Pay 25,000 for each house and hotel for repears</t>
+  </si>
+  <si>
+    <t>Go for a reading. Advance 10 blocks</t>
+  </si>
+  <si>
+    <t>You broke your leg sking. Pay 100,000 for medical expenses</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Get Money</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Go to jail</t>
+  </si>
+  <si>
+    <t>Pay</t>
   </si>
 </sst>
 </file>
@@ -472,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DC18AB-49CE-40CD-AD88-5FED76798156}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,4 +1076,470 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EB29BE-B85D-4B43-9474-4CF4E2E0C2ED}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>200000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>100000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>200000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC703184-D97E-445B-8A66-6DDD4B7A10EE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>250000</v>
+      </c>
+      <c r="C2">
+        <v>75000</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>250000</v>
+      </c>
+      <c r="C3">
+        <v>75000</v>
+      </c>
+      <c r="D3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>250000</v>
+      </c>
+      <c r="C4">
+        <v>75000</v>
+      </c>
+      <c r="D4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>250000</v>
+      </c>
+      <c r="C5">
+        <v>75000</v>
+      </c>
+      <c r="D5">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207E4606-DB34-4B89-940E-3B43FA1D5C77}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>250000</v>
+      </c>
+      <c r="C2">
+        <v>75000</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>250000</v>
+      </c>
+      <c r="C3">
+        <v>75000</v>
+      </c>
+      <c r="D3">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578FAF8D-EEA7-47F3-B8CC-B7B17D7FE4D3}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3A002C-5B1D-4BBC-9C22-2A6B535795B6}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="63.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed all cards classes
</commit_message>
<xml_diff>
--- a/Monopoly_data.xlsx
+++ b/Monopoly_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Desktop\CS projects\Python_Programs\github_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F642531-A545-4A80-BFE2-86C0E67BAF2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AFDF70-802E-412A-8909-AD5FCAF70A87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D6DA0972-7B55-441C-8D73-5E4A5A098029}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{D6DA0972-7B55-441C-8D73-5E4A5A098029}"/>
   </bookViews>
   <sheets>
     <sheet name="European Cities" sheetId="1" r:id="rId1"/>
@@ -1183,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC703184-D97E-445B-8A66-6DDD4B7A10EE}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -1335,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578FAF8D-EEA7-47F3-B8CC-B7B17D7FE4D3}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Completed all cards classes and populate in dictionaries
</commit_message>
<xml_diff>
--- a/Monopoly_data.xlsx
+++ b/Monopoly_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Desktop\CS projects\Python_Programs\github_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AFDF70-802E-412A-8909-AD5FCAF70A87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F98FB3-301A-4E7E-A37A-9373E964A93D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{D6DA0972-7B55-441C-8D73-5E4A5A098029}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
     <t>City</t>
   </si>
@@ -161,12 +161,6 @@
     <t>Card</t>
   </si>
   <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>Chance</t>
-  </si>
-  <si>
     <t>Money Lost</t>
   </si>
   <si>
@@ -246,16 +240,91 @@
   </si>
   <si>
     <t>Pay</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Chance1</t>
+  </si>
+  <si>
+    <t>Chance2</t>
+  </si>
+  <si>
+    <t>Chance3</t>
+  </si>
+  <si>
+    <t>Chance4</t>
+  </si>
+  <si>
+    <t>Chance5</t>
+  </si>
+  <si>
+    <t>Chance6</t>
+  </si>
+  <si>
+    <t>Chance7</t>
+  </si>
+  <si>
+    <t>Chance8</t>
+  </si>
+  <si>
+    <t>Chance9</t>
+  </si>
+  <si>
+    <t>Chance10</t>
+  </si>
+  <si>
+    <t>Community1</t>
+  </si>
+  <si>
+    <t>Community2</t>
+  </si>
+  <si>
+    <t>Community3</t>
+  </si>
+  <si>
+    <t>Community4</t>
+  </si>
+  <si>
+    <t>Community5</t>
+  </si>
+  <si>
+    <t>Community6</t>
+  </si>
+  <si>
+    <t>Community7</t>
+  </si>
+  <si>
+    <t>Community8</t>
+  </si>
+  <si>
+    <t>Community9</t>
+  </si>
+  <si>
+    <t>Community10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1083,7 +1152,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,16 +1162,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1113,7 +1182,7 @@
         <v>200000</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1135,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1146,12 +1215,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1160,18 +1229,18 @@
         <v>100000</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>200000</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1253,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1264,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1273,7 +1342,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,7 +1355,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1336,7 +1405,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,90 +1419,91 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1443,11 +1513,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="29.77734375" customWidth="1"/>
     <col min="2" max="2" width="63.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1456,90 +1527,91 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>